<commit_message>
Enhance Azure DevOps integration and improve chatbot functionality
</commit_message>
<xml_diff>
--- a/Back End/work_items_due_dates.xlsx
+++ b/Back End/work_items_due_dates.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -42,21 +42,18 @@
     <t>Severity</t>
   </si>
   <si>
+    <t>TEST_02: Something</t>
+  </si>
+  <si>
+    <t>TEST_01: Introduction</t>
+  </si>
+  <si>
     <t>TEST_05: Strawberry</t>
   </si>
   <si>
     <t>TEST_04: Testing Sandwiches</t>
   </si>
   <si>
-    <t>TEST_03: Coffee Cake</t>
-  </si>
-  <si>
-    <t>TEST_02: Something</t>
-  </si>
-  <si>
-    <t>TEST_01: Introduction</t>
-  </si>
-  <si>
     <t>Creating BRD</t>
   </si>
   <si>
@@ -69,39 +66,36 @@
     <t>Gather Design</t>
   </si>
   <si>
+    <t>In Progress</t>
+  </si>
+  <si>
     <t>New</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Kenneth Kui</t>
   </si>
   <si>
+    <t>Priththiha Nemikumar</t>
+  </si>
+  <si>
     <t>Kamini Patel</t>
   </si>
   <si>
+    <t>2024-12-03T00:00:00Z</t>
+  </si>
+  <si>
+    <t>2024-12-02T00:00:00Z</t>
+  </si>
+  <si>
     <t>2024-12-06T00:00:00Z</t>
   </si>
   <si>
     <t>2024-12-05T00:00:00Z</t>
   </si>
   <si>
-    <t>2024-12-04T00:00:00Z</t>
-  </si>
-  <si>
-    <t>2024-12-03T00:00:00Z</t>
-  </si>
-  <si>
-    <t>2024-12-02T00:00:00Z</t>
-  </si>
-  <si>
     <t>Preet Patel</t>
   </si>
   <si>
-    <t>QA | Sure, whatever</t>
-  </si>
-  <si>
     <t>Something something</t>
   </si>
   <si>
@@ -111,12 +105,12 @@
     <t>Bug | Critical | Login Error</t>
   </si>
   <si>
+    <t>2024-12-07T00:00:00Z</t>
+  </si>
+  <si>
     <t>2024-12-13T00:00:00Z</t>
   </si>
   <si>
-    <t>2024-12-07T00:00:00Z</t>
-  </si>
-  <si>
     <t>2024-12-12T00:00:00Z</t>
   </si>
   <si>
@@ -144,10 +138,7 @@
     <t>Bug | Major | Backend Failure</t>
   </si>
   <si>
-    <t>Arian Fooladray</t>
-  </si>
-  <si>
-    <t>Priththiha Nemikumar</t>
+    <t>afooladray@fgfbrands.com</t>
   </si>
   <si>
     <t>2024-12-20T00:00:00Z</t>
@@ -517,7 +508,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -551,19 +542,22 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -571,22 +565,22 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
         <v>22</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -594,13 +588,13 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
@@ -609,7 +603,7 @@
         <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -617,22 +611,22 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -640,7 +634,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6">
-        <v>984</v>
+        <v>992</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -649,13 +643,13 @@
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -663,22 +657,22 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -686,22 +680,22 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8">
-        <v>990</v>
+        <v>1005</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8">
         <v>2</v>
@@ -709,47 +703,24 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9">
-        <v>1005</v>
+        <v>991</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10">
-        <v>991</v>
-      </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10">
         <v>2</v>
       </c>
     </row>
@@ -760,7 +731,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -794,48 +765,45 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>945</v>
+        <v>993</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2">
         <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3">
-        <v>993</v>
+        <v>1006</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -843,51 +811,28 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4">
-        <v>1006</v>
+        <v>960</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
         <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
-        <v>960</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5">
         <v>1</v>
       </c>
-      <c r="H5" t="s">
-        <v>34</v>
+      <c r="H4" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -934,25 +879,25 @@
         <v>940</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2">
         <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -960,25 +905,25 @@
         <v>926</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -986,25 +931,25 @@
         <v>927</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1012,25 +957,25 @@
         <v>929</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1038,25 +983,25 @@
         <v>930</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6">
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1064,25 +1009,25 @@
         <v>933</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1090,25 +1035,25 @@
         <v>934</v>
       </c>
       <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>40</v>
       </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>42</v>
-      </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8">
         <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1116,25 +1061,25 @@
         <v>932</v>
       </c>
       <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" t="s">
-        <v>44</v>
-      </c>
       <c r="F9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9">
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1142,25 +1087,25 @@
         <v>931</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10">
         <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1168,25 +1113,25 @@
         <v>928</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>